<commit_message>
Updated sprint backlog/Added burndownChart
</commit_message>
<xml_diff>
--- a/Phase 2/Sprint2/Sprint backlog.xlsx
+++ b/Phase 2/Sprint2/Sprint backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dany5\Desktop\SE2223_59797_60441_60677_60816_60971\Phase 2\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41921EEA-8DA9-4684-B322-CCB453838419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA73283-2848-42D6-9511-6E34D6B6FA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F947D5B0-1B2A-0145-ADC6-725523378344}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TO DO</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Escolher duas ideias</t>
+  </si>
+  <si>
+    <t>Estudar aplicação</t>
   </si>
 </sst>
 </file>
@@ -106,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -131,15 +134,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -192,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,16 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -233,11 +218,17 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -258,106 +249,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Conexão reta 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31F31418-294C-7E70-BF2B-D94FF9B598C4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8286750" y="619125"/>
-          <a:ext cx="1390650" cy="590550"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Conexão reta 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E376696B-B4A7-6C57-C8E9-F20BCAF12E2A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8296275" y="619125"/>
-          <a:ext cx="1371600" cy="600075"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -439,11 +330,107 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conexão reta 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3AD0203-972C-6923-64F4-2AC6018DF9A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8296275" y="590550"/>
+          <a:ext cx="1390650" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conexão reta 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F3F5506-28FE-3992-C835-E5E6B0C45E49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8286750" y="609600"/>
+          <a:ext cx="1381125" cy="790575"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -746,7 +733,7 @@
   <dimension ref="A3:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -755,63 +742,65 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="E3" s="13" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="E3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="8" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="E6" s="12" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="E7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="7"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E8" s="4"/>
@@ -857,7 +846,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G4:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>